<commit_message>
Continuing to work on supplementary
</commit_message>
<xml_diff>
--- a/Proj0_SupplementaryTables.xlsx
+++ b/Proj0_SupplementaryTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lmee/Documents/Projects/ProjectZero/Proj0_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FBEFA8-8DC4-B248-AE34-B31818E4DA14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219C4D0A-DB3D-354C-9810-06713C324436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="7" xr2:uid="{076ED038-645B-EB45-B69E-87D41BCFAF89}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" firstSheet="1" activeTab="6" xr2:uid="{076ED038-645B-EB45-B69E-87D41BCFAF89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="NonCanon_BP_GOterms" sheetId="3" r:id="rId3"/>
     <sheet name="NonCanon_MF_GOterms" sheetId="6" r:id="rId4"/>
     <sheet name="NonCanon_CC_GOterms" sheetId="5" r:id="rId5"/>
-    <sheet name="Random_BP_GOterms" sheetId="7" r:id="rId6"/>
-    <sheet name="Random_MF_GOterms" sheetId="8" r:id="rId7"/>
-    <sheet name="Random_CC_GOterms" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="11" r:id="rId6"/>
+    <sheet name="Random_BP_GOterms" sheetId="7" r:id="rId7"/>
+    <sheet name="Random_MF_GOterms" sheetId="8" r:id="rId8"/>
+    <sheet name="Random_CC_GOterms" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="1956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2782" uniqueCount="1967">
   <si>
     <t>p.value</t>
   </si>
@@ -5909,6 +5910,39 @@
   </si>
   <si>
     <t xml:space="preserve"> "mitochondrial proton-transporting ATP synthase complex, coupling factor F(o)"</t>
+  </si>
+  <si>
+    <t>Overlaps</t>
+  </si>
+  <si>
+    <t>Adv and Soc</t>
+  </si>
+  <si>
+    <t>Adv and Sol</t>
+  </si>
+  <si>
+    <t>Sol and Soc</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>NonCanon</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Api and Hali</t>
+  </si>
+  <si>
+    <t>Hali and Mega</t>
+  </si>
+  <si>
+    <t>Mega and Api</t>
+  </si>
+  <si>
+    <t>immune</t>
   </si>
 </sst>
 </file>
@@ -5979,10 +6013,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6325,30 +6359,30 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="11"/>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="11"/>
       <c r="J5" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="L5" t="s">
@@ -6356,7 +6390,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="11"/>
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -6366,7 +6400,7 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="11"/>
       <c r="F6" t="s">
         <v>9</v>
       </c>
@@ -6379,7 +6413,7 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="11"/>
       <c r="L6" t="s">
         <v>9</v>
       </c>
@@ -7002,10 +7036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A65D2F-0E09-6140-BC98-DF7EEC89AF19}">
-  <dimension ref="A5:I175"/>
+  <dimension ref="A3:K175"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7016,24 +7050,37 @@
     <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="K5" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -7061,8 +7108,11 @@
       <c r="I6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -7090,8 +7140,11 @@
       <c r="I7">
         <v>0.46700000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -7110,8 +7163,11 @@
       <c r="F8">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -7130,8 +7186,11 @@
       <c r="F9">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -7150,8 +7209,11 @@
       <c r="F10">
         <v>1.401</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -7170,8 +7232,11 @@
       <c r="F11">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -7190,8 +7255,11 @@
       <c r="F12">
         <v>1.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -7210,8 +7278,11 @@
       <c r="F13">
         <v>2.5999999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -7230,8 +7301,11 @@
       <c r="F14">
         <v>0.317</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -7250,8 +7324,11 @@
       <c r="F15">
         <v>0.23799999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -7270,8 +7347,11 @@
       <c r="F16">
         <v>0.33500000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -7290,8 +7370,11 @@
       <c r="F17">
         <v>0.626</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -7310,8 +7393,11 @@
       <c r="F18">
         <v>1.974</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -7330,8 +7416,11 @@
       <c r="F19">
         <v>0.48499999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -7350,8 +7439,11 @@
       <c r="F20">
         <v>1.542</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -7371,7 +7463,7 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -7391,7 +7483,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -7411,7 +7503,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -7431,7 +7523,7 @@
         <v>0.159</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -7451,7 +7543,7 @@
         <v>1.956</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -7471,7 +7563,7 @@
         <v>1.9390000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>83</v>
       </c>
@@ -7491,7 +7583,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -7511,7 +7603,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -7531,7 +7623,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -7551,7 +7643,7 @@
         <v>0.22900000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -7571,7 +7663,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -7737,19 +7829,19 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10" t="s">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -8546,21 +8638,21 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B105" s="10"/>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10" t="s">
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E105" s="10"/>
-      <c r="F105" s="10"/>
-      <c r="G105" s="10" t="s">
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H105" s="10"/>
-      <c r="I105" s="10"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -9120,21 +9212,21 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A147" s="10" t="s">
+      <c r="A147" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B147" s="10"/>
-      <c r="C147" s="10"/>
-      <c r="D147" s="10" t="s">
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E147" s="10"/>
-      <c r="F147" s="10"/>
-      <c r="G147" s="10" t="s">
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+      <c r="G147" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H147" s="10"/>
-      <c r="I147" s="10"/>
+      <c r="H147" s="11"/>
+      <c r="I147" s="11"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
@@ -9644,18 +9736,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="G48:I48"/>
     <mergeCell ref="A105:C105"/>
     <mergeCell ref="D105:F105"/>
     <mergeCell ref="G105:I105"/>
     <mergeCell ref="A147:C147"/>
     <mergeCell ref="D147:F147"/>
     <mergeCell ref="G147:I147"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="G48:I48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9665,8 +9757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60042974-8ABF-AA46-BC7D-4D42AA38BFAA}">
   <dimension ref="A5:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9678,21 +9770,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -9855,16 +9947,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -10306,32 +10398,32 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10" t="s">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10" t="s">
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -10643,21 +10735,21 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10" t="s">
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
-      <c r="G69" s="10" t="s">
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -10969,6 +11061,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="A69:C69"/>
     <mergeCell ref="D69:F69"/>
     <mergeCell ref="G69:I69"/>
@@ -10978,11 +11075,6 @@
     <mergeCell ref="G43:I43"/>
     <mergeCell ref="D43:F43"/>
     <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10993,7 +11085,7 @@
   <dimension ref="A5:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+      <selection activeCell="J12" sqref="J12:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11005,21 +11097,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -11266,16 +11358,16 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -11430,7 +11522,7 @@
       <c r="D29" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>153</v>
       </c>
       <c r="F29">
@@ -11522,21 +11614,21 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10" t="s">
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10" t="s">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -11749,21 +11841,21 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10" t="s">
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10" t="s">
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -11973,28 +12065,690 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="G37:I37"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="D54:F54"/>
     <mergeCell ref="G54:I54"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069D888F-5B03-1A4C-8D96-320F0DF037CD}">
+  <dimension ref="A1:M60"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M52" sqref="M2:M52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1956</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1961</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1962</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1958</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1959</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1957</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1958</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1959</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1960</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" t="s">
+        <v>539</v>
+      </c>
+      <c r="F4" t="s">
+        <v>761</v>
+      </c>
+      <c r="G4" t="s">
+        <v>982</v>
+      </c>
+      <c r="H4" t="s">
+        <v>851</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>575</v>
+      </c>
+      <c r="F5" t="s">
+        <v>978</v>
+      </c>
+      <c r="G5" t="s">
+        <v>984</v>
+      </c>
+      <c r="H5" t="s">
+        <v>894</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C6" t="s">
+        <v>579</v>
+      </c>
+      <c r="F6" t="s">
+        <v>841</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1253</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>365</v>
+      </c>
+      <c r="C7" t="s">
+        <v>496</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1265</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>398</v>
+      </c>
+      <c r="F8" t="s">
+        <v>908</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>409</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1416</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>421</v>
+      </c>
+      <c r="F10" t="s">
+        <v>847</v>
+      </c>
+      <c r="G10" t="s">
+        <v>805</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1561</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1057</v>
+      </c>
+      <c r="H11" t="s">
+        <v>271</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>448</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1469</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>225</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1471</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1473</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1483</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>361</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1515</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1333</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1339</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>252</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>258</v>
+      </c>
+      <c r="M20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>277</v>
+      </c>
+      <c r="M21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>433</v>
+      </c>
+      <c r="M22" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>435</v>
+      </c>
+      <c r="M23" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="M24" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>146</v>
+      </c>
+      <c r="M25" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>162</v>
+      </c>
+      <c r="M27" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>164</v>
+      </c>
+      <c r="M28" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="M29" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>450</v>
+      </c>
+      <c r="M30" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M31" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>1963</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1964</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1965</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1960</v>
+      </c>
+      <c r="M32" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>761</v>
+      </c>
+      <c r="G33" t="s">
+        <v>571</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1265</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1253</v>
+      </c>
+      <c r="M33" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="34" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>978</v>
+      </c>
+      <c r="H34" t="s">
+        <v>851</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1333</v>
+      </c>
+      <c r="M34" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H35" t="s">
+        <v>894</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="36" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1339</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1081</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="38" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>1357</v>
+      </c>
+      <c r="M38" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="39" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>1664</v>
+      </c>
+      <c r="M39" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="40" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>1586</v>
+      </c>
+      <c r="M40" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="41" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>1394</v>
+      </c>
+      <c r="M41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F42" t="s">
+        <v>1602</v>
+      </c>
+      <c r="M42" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="43" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>1416</v>
+      </c>
+      <c r="M43" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="44" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>1582</v>
+      </c>
+      <c r="M44" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="45" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
+        <v>1057</v>
+      </c>
+      <c r="M45" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="46" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F46" t="s">
+        <v>1059</v>
+      </c>
+      <c r="M46" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="47" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F47" t="s">
+        <v>1191</v>
+      </c>
+      <c r="M47" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="48" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>1211</v>
+      </c>
+      <c r="M48" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="49" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>1331</v>
+      </c>
+      <c r="M49" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="50" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>1341</v>
+      </c>
+      <c r="M50" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="51" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
+        <v>1471</v>
+      </c>
+      <c r="M51" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="52" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F52" t="s">
+        <v>1473</v>
+      </c>
+      <c r="M52" t="s">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="53" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="54" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="55" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F55" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="56" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="57" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="58" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="59" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="60" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8E0976-FD17-BE43-8553-D3DE1ECB6CC3}">
   <dimension ref="A5:K222"/>
   <sheetViews>
-    <sheetView topLeftCell="B168" workbookViewId="0">
-      <selection activeCell="H202" sqref="H202"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12006,21 +12760,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -12716,7 +13470,7 @@
       <c r="D30" t="s">
         <v>890</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>891</v>
       </c>
       <c r="F30">
@@ -12872,16 +13626,16 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10" t="s">
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
@@ -13844,21 +14598,21 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10"/>
-      <c r="D96" s="10" t="s">
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10" t="s">
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H96" s="10"/>
-      <c r="I96" s="10"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
@@ -15091,22 +15845,22 @@
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A164" s="10" t="s">
+      <c r="A164" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B164" s="10"/>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10" t="s">
+      <c r="B164" s="11"/>
+      <c r="C164" s="11"/>
+      <c r="D164" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E164" s="10"/>
-      <c r="F164" s="10"/>
-      <c r="G164" s="10" t="s">
+      <c r="E164" s="11"/>
+      <c r="F164" s="11"/>
+      <c r="G164" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H164" s="10"/>
-      <c r="I164" s="10"/>
-      <c r="J164" s="10"/>
+      <c r="H164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11"/>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
@@ -16495,6 +17249,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
     <mergeCell ref="A164:C164"/>
     <mergeCell ref="D164:F164"/>
     <mergeCell ref="G164:J164"/>
@@ -16503,20 +17260,17 @@
     <mergeCell ref="A96:C96"/>
     <mergeCell ref="D96:F96"/>
     <mergeCell ref="G96:I96"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3177DF09-A060-DF49-BE7C-5A48CE186D61}">
   <dimension ref="A5:I110"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86:I102"/>
+    <sheetView topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16528,21 +17282,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -16798,16 +17552,16 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -17254,21 +18008,21 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10" t="s">
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -17743,9 +18497,9 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
       <c r="D77" t="s">
         <v>1511</v>
       </c>
@@ -17812,21 +18566,21 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10" t="s">
+      <c r="B84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10" t="s">
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H84" s="10"/>
-      <c r="I84" s="10"/>
+      <c r="H84" s="11"/>
+      <c r="I84" s="11"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -18513,17 +19267,17 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="A84:C84"/>
     <mergeCell ref="D84:F84"/>
     <mergeCell ref="G84:I84"/>
     <mergeCell ref="A47:C47"/>
     <mergeCell ref="D47:F47"/>
     <mergeCell ref="G47:I47"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
     <mergeCell ref="A77:C77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18531,12 +19285,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E952499-56AE-0C4D-8EC5-8F51CF47F066}">
   <dimension ref="A5:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60:K70"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18548,21 +19302,21 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -18720,16 +19474,16 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -18987,21 +19741,21 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -19382,21 +20136,21 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10" t="s">
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10" t="s">
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">

</xml_diff>